<commit_message>
basic graph data visible but not aligned with columns. fixed data where a dose had the wrong prescrition
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/doses.xlsx
+++ b/src/main/resources/initialDataFiles/doses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catha\Documents\Health\ADHD\medTrackerInitialData\Personal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2873C4-1942-42C3-A5DA-2E5EDC0208DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9506A6-2AD6-4621-9C5E-61029CD0FCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3010" yWindow="-110" windowWidth="35500" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,8 +368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,7 +803,7 @@
         <v>45597</v>
       </c>
       <c r="B31" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
inital data prescription should reference user id 4 use all medications and day stages from prescriptions rather than doses
</commit_message>
<xml_diff>
--- a/src/main/resources/initialDataFiles/doses.xlsx
+++ b/src/main/resources/initialDataFiles/doses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\initialDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9506A6-2AD6-4621-9C5E-61029CD0FCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9159A2-152B-4D17-BDAA-8D82B5BAEA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-60" windowWidth="35200" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3010" yWindow="-110" windowWidth="35500" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,11 +81,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1400,9 +1401,93 @@
         <v>0.59375</v>
       </c>
     </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B74" s="1">
+        <v>8</v>
+      </c>
+      <c r="C74" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74" s="3">
+        <v>0.4236111111111111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="2">
+        <v>45626</v>
+      </c>
+      <c r="B75" s="1">
+        <v>9</v>
+      </c>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75" s="3">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="2">
+        <v>45627</v>
+      </c>
+      <c r="B76" s="1">
+        <v>8</v>
+      </c>
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" s="3">
+        <v>0.4236111111111111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="2">
+        <v>45627</v>
+      </c>
+      <c r="B77" s="1">
+        <v>9</v>
+      </c>
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" s="3">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="2">
+        <v>45628</v>
+      </c>
+      <c r="B78" s="1">
+        <v>8</v>
+      </c>
+      <c r="C78" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="2">
+        <v>45628</v>
+      </c>
+      <c r="B79" s="1">
+        <v>9</v>
+      </c>
+      <c r="C79" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" s="4">
+        <v>0.59166666666666667</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
-    <sortCondition ref="A2:A73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A74:D79">
+    <sortCondition ref="A74:A79"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>